<commit_message>
corrected doc weight to 4
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen_P56_HS18.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen_P56_HS18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de\Source\Repos\ProStudCreator\ProStudCreator\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5DF05015-E449-464A-A301-96A858D7B3BE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{78E13221-4028-4392-938B-D599CD45D04E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5265" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -1643,9 +1643,51 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1684,48 +1726,6 @@
     </xf>
     <xf numFmtId="14" fontId="23" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5223,160 +5223,160 @@
       <c r="A8" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
+      <c r="B8" s="163"/>
+      <c r="C8" s="163"/>
     </row>
     <row r="9" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="177"/>
-      <c r="C9" s="178"/>
+      <c r="B9" s="164"/>
+      <c r="C9" s="165"/>
     </row>
     <row r="10" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="61"/>
-      <c r="B10" s="179"/>
-      <c r="C10" s="180"/>
+      <c r="B10" s="166"/>
+      <c r="C10" s="167"/>
     </row>
     <row r="11" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="176"/>
-      <c r="C11" s="176"/>
+      <c r="B11" s="163"/>
+      <c r="C11" s="163"/>
     </row>
     <row r="12" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
+      <c r="B12" s="163"/>
+      <c r="C12" s="163"/>
     </row>
     <row r="13" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="55"/>
       <c r="B13" s="56"/>
     </row>
     <row r="14" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="168"/>
-      <c r="C14" s="169"/>
+      <c r="B14" s="154"/>
+      <c r="C14" s="155"/>
     </row>
     <row r="15" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="170"/>
-      <c r="B15" s="171"/>
-      <c r="C15" s="172"/>
+      <c r="A15" s="156"/>
+      <c r="B15" s="157"/>
+      <c r="C15" s="158"/>
     </row>
     <row r="16" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="170"/>
-      <c r="B16" s="171"/>
-      <c r="C16" s="172"/>
+      <c r="A16" s="156"/>
+      <c r="B16" s="157"/>
+      <c r="C16" s="158"/>
     </row>
     <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="170"/>
-      <c r="B17" s="171"/>
-      <c r="C17" s="172"/>
+      <c r="A17" s="156"/>
+      <c r="B17" s="157"/>
+      <c r="C17" s="158"/>
     </row>
     <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="170"/>
-      <c r="B18" s="171"/>
-      <c r="C18" s="172"/>
+      <c r="A18" s="156"/>
+      <c r="B18" s="157"/>
+      <c r="C18" s="158"/>
     </row>
     <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="170"/>
-      <c r="B19" s="171"/>
-      <c r="C19" s="172"/>
+      <c r="A19" s="156"/>
+      <c r="B19" s="157"/>
+      <c r="C19" s="158"/>
     </row>
     <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="170"/>
-      <c r="B20" s="171"/>
-      <c r="C20" s="172"/>
+      <c r="A20" s="156"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="158"/>
     </row>
     <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="170"/>
-      <c r="B21" s="171"/>
-      <c r="C21" s="172"/>
+      <c r="A21" s="156"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="158"/>
     </row>
     <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="170"/>
-      <c r="B22" s="171"/>
-      <c r="C22" s="172"/>
+      <c r="A22" s="156"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="158"/>
     </row>
     <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="170"/>
-      <c r="B23" s="171"/>
-      <c r="C23" s="172"/>
+      <c r="A23" s="156"/>
+      <c r="B23" s="157"/>
+      <c r="C23" s="158"/>
     </row>
     <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="170"/>
-      <c r="B24" s="171"/>
-      <c r="C24" s="172"/>
+      <c r="A24" s="156"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="158"/>
     </row>
     <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="170"/>
-      <c r="B25" s="171"/>
-      <c r="C25" s="172"/>
+      <c r="A25" s="156"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="158"/>
     </row>
     <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="170"/>
-      <c r="B26" s="171"/>
-      <c r="C26" s="172"/>
+      <c r="A26" s="156"/>
+      <c r="B26" s="157"/>
+      <c r="C26" s="158"/>
     </row>
     <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="170"/>
-      <c r="B27" s="171"/>
-      <c r="C27" s="172"/>
+      <c r="A27" s="156"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="158"/>
     </row>
     <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="170"/>
-      <c r="B28" s="171"/>
-      <c r="C28" s="172"/>
+      <c r="A28" s="156"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="158"/>
     </row>
     <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="170"/>
-      <c r="B29" s="171"/>
-      <c r="C29" s="172"/>
+      <c r="A29" s="156"/>
+      <c r="B29" s="157"/>
+      <c r="C29" s="158"/>
     </row>
     <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="170"/>
-      <c r="B30" s="171"/>
-      <c r="C30" s="172"/>
+      <c r="A30" s="156"/>
+      <c r="B30" s="157"/>
+      <c r="C30" s="158"/>
     </row>
     <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="170"/>
-      <c r="B31" s="171"/>
-      <c r="C31" s="172"/>
+      <c r="A31" s="156"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="158"/>
     </row>
     <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="170"/>
-      <c r="B32" s="171"/>
-      <c r="C32" s="172"/>
+      <c r="A32" s="156"/>
+      <c r="B32" s="157"/>
+      <c r="C32" s="158"/>
     </row>
     <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="170"/>
-      <c r="B33" s="171"/>
-      <c r="C33" s="172"/>
+      <c r="A33" s="156"/>
+      <c r="B33" s="157"/>
+      <c r="C33" s="158"/>
     </row>
     <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="170"/>
-      <c r="B34" s="171"/>
-      <c r="C34" s="172"/>
+      <c r="A34" s="156"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="158"/>
     </row>
     <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="173"/>
-      <c r="B35" s="174"/>
-      <c r="C35" s="175"/>
+      <c r="A35" s="159"/>
+      <c r="B35" s="160"/>
+      <c r="C35" s="161"/>
     </row>
     <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="55"/>
       <c r="B36" s="56"/>
     </row>
     <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="153" t="s">
+      <c r="A37" s="162" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="153"/>
+      <c r="B37" s="162"/>
       <c r="C37" s="62">
         <f>'2. Detailbewertung (Excel)'!C34</f>
         <v>4.4000000000000004</v>
@@ -5387,30 +5387,30 @@
       <c r="B38" s="56"/>
     </row>
     <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="153" t="s">
+      <c r="A39" s="162" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="153"/>
-      <c r="C39" s="153"/>
+      <c r="B39" s="162"/>
+      <c r="C39" s="162"/>
     </row>
     <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="159" t="s">
+      <c r="A40" s="173" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="160"/>
-      <c r="C40" s="161"/>
+      <c r="B40" s="174"/>
+      <c r="C40" s="175"/>
     </row>
     <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="162"/>
-      <c r="B41" s="163"/>
-      <c r="C41" s="164"/>
+      <c r="A41" s="176"/>
+      <c r="B41" s="177"/>
+      <c r="C41" s="178"/>
     </row>
     <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="154" t="s">
+      <c r="A42" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="154"/>
-      <c r="C42" s="154"/>
+      <c r="B42" s="168"/>
+      <c r="C42" s="168"/>
     </row>
     <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="55"/>
@@ -5424,54 +5424,48 @@
       <c r="A45" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="165">
+      <c r="B45" s="179">
         <f ca="1">TODAY()</f>
         <v>43297</v>
       </c>
-      <c r="C45" s="166"/>
+      <c r="C45" s="180"/>
     </row>
     <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="58"/>
-      <c r="B46" s="155"/>
-      <c r="C46" s="155"/>
+      <c r="B46" s="169"/>
+      <c r="C46" s="169"/>
     </row>
     <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="58"/>
-      <c r="B47" s="155"/>
-      <c r="C47" s="155"/>
+      <c r="B47" s="169"/>
+      <c r="C47" s="169"/>
     </row>
     <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="155"/>
-      <c r="C48" s="155"/>
+      <c r="B48" s="169"/>
+      <c r="C48" s="169"/>
     </row>
     <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="59"/>
-      <c r="B49" s="155"/>
-      <c r="C49" s="155"/>
+      <c r="B49" s="169"/>
+      <c r="C49" s="169"/>
     </row>
     <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="156"/>
-      <c r="C50" s="156"/>
+      <c r="B50" s="170"/>
+      <c r="C50" s="170"/>
     </row>
     <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="60"/>
-      <c r="B51" s="157"/>
-      <c r="C51" s="158"/>
+      <c r="B51" s="171"/>
+      <c r="C51" s="172"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A14:C35"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B9:C10"/>
     <mergeCell ref="A39:C39"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="B49:C49"/>
@@ -5482,6 +5476,12 @@
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="B48:C48"/>
+    <mergeCell ref="A14:C35"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B9:C10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.68" right="0.19" top="0.25" bottom="0.97" header="0.96" footer="0.4921259845"/>
@@ -5496,7 +5496,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5798,7 +5798,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="97">
         <v>6</v>
@@ -5859,7 +5859,7 @@
       </c>
       <c r="D22" s="115">
         <f>(C19*D19+C20*D20+C21*D21)/SUM(C19:C21)</f>
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="E22" s="43"/>
       <c r="F22" s="44"/>
@@ -5962,7 +5962,7 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119">
         <f>(C10*D10+C17*D17+C22*D22+C27*D27)/SUM(C10,C17,C22,C27)</f>
-        <v>4.2583333333333329</v>
+        <v>4.3</v>
       </c>
       <c r="E28" s="45"/>
       <c r="F28" s="46"/>

</xml_diff>

<commit_message>
Bewertungsbogen weights -> DG modell
</commit_message>
<xml_diff>
--- a/ProStudCreator/Content/Bewertungsbogen_P56_HS18.xlsx
+++ b/ProStudCreator/Content/Bewertungsbogen_P56_HS18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\de\Source\Repos\ProStudCreator\ProStudCreator\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{78E13221-4028-4392-938B-D599CD45D04E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{887E4B21-8AA1-4225-B98F-0E4C23562F20}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5265" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7425" yWindow="1035" windowWidth="15480" windowHeight="11640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Gesamtbewertung (Text)" sheetId="2" r:id="rId1"/>
@@ -223,31 +223,10 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Analyse von  Ergebnissen</t>
-  </si>
-  <si>
-    <t>Selbstständigkeit / Betreuungsintensität</t>
-  </si>
-  <si>
     <t>Projektvereinbarung Inhalt</t>
   </si>
   <si>
     <t>Projektvereinbarung Projektplanung</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lösungskonzept / Strategie
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Je nach Komplexität der Aufgabenstellung soll die Gewichtung zwischen 0.2 (einfach) und 1 (komplex) liegen.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -325,32 +304,10 @@
     </r>
   </si>
   <si>
-    <t>DOKUMENTATION,  WISSENSTRANSFER</t>
-  </si>
-  <si>
     <t>GESAMTNOTE</t>
   </si>
   <si>
     <t>Bewertungsbogen: Projektarbeit 5 und Bachelorthesis (Projektarbeit 6)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Bemerkungen:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Dieser Bewertungsbogen wird von der betreunden Person ausgefüllt. Bei zwei betreuenden Personen wird er von beiden unabhängig ausgefüllt und danach abgeglichen. Wo möglich und sinnvoll wird ein Kommentar zu jeder Bewertung verfasst. Die Studierenden erhalten in jedem Fall die Würdigung in Papierform. Falls erwünscht wird auch der Bewertungsbogen in PDF From abgegeben. Nach der Projektarbeit 5 muss dieser Bewertungsbogen zwingen mit den Studierenden besprochen und auf mögliches Verbesserungspotential für die kommende Projektarbeit 6 hingewiesen werden. Nach Abschluss der Projektarbeit 6 wird der Bewertungsbogen auf Wunsch der Studierenden mit diesen besprochen.</t>
-    </r>
   </si>
   <si>
     <t>Kommunikation der Bewertung</t>
@@ -384,6 +341,49 @@
   </si>
   <si>
     <t>Das Blatt "2. Detailbewertung" wird ebenfalls an die Studierenden abgegeben, ggf. aber ohne die Kommentare (Spalte G). Die Teilnoten (Spalte D) werden abgegeben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Analyse von Ergebnissen</t>
+  </si>
+  <si>
+    <t>DOKUMENTATION, WISSENSTRANSFER</t>
+  </si>
+  <si>
+    <t>Selbstständigkeit/Betreuungsintensität</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lösungskonzept/Strategie
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Je nach Komplexität der Aufgabenstellung soll die Gewichtung zwischen 0.2 (einfach) und 1 (komplex) liegen.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Bemerkungen:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Dieser Bewertungsbogen wird von der betreunden Person ausgefüllt. Bei zwei betreuenden Personen wird er von beiden unabhängig ausgefüllt und danach abgeglichen. Wo möglich und sinnvoll wird ein Kommentar zu jeder Bewertung verfasst. Die Studierenden erhalten in jedem Fall die Würdigung in Papierform. Falls erwünscht wird auch der Bewertungsbogen in PDF-Form abgegeben. Nach der Projektarbeit 5 muss dieser Bewertungsbogen zwingen mit den Studierenden besprochen und auf mögliches Verbesserungspotential für die kommende Projektarbeit 6 hingewiesen werden. Nach Abschluss der Projektarbeit 6 wird der Bewertungsbogen auf Wunsch der Studierenden mit diesen besprochen.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -5204,7 +5204,7 @@
   <dimension ref="A6:C51"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5379,7 +5379,7 @@
       <c r="B37" s="162"/>
       <c r="C37" s="62">
         <f>'2. Detailbewertung (Excel)'!C34</f>
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="B45" s="179">
         <f ca="1">TODAY()</f>
-        <v>43297</v>
+        <v>43322</v>
       </c>
       <c r="C45" s="180"/>
     </row>
@@ -5496,7 +5496,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5512,7 +5512,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="127" customFormat="1" ht="29.65" x14ac:dyDescent="0.65">
       <c r="B1" s="130" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C1" s="129"/>
       <c r="D1" s="129"/>
@@ -5531,7 +5531,7 @@
     </row>
     <row r="3" spans="1:7" ht="114" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="181" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C3" s="181"/>
       <c r="D3" s="181"/>
@@ -5573,7 +5573,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="192" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C6" s="193"/>
       <c r="D6" s="193"/>
@@ -5586,14 +5586,12 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C7" s="95">
         <v>0.5</v>
       </c>
-      <c r="D7" s="96">
-        <v>4</v>
-      </c>
+      <c r="D7" s="96"/>
       <c r="E7" s="27"/>
       <c r="F7" s="28" t="s">
         <v>31</v>
@@ -5605,14 +5603,12 @@
         <v>1.2</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="124">
         <v>1</v>
       </c>
-      <c r="D8" s="97">
-        <v>4.5</v>
-      </c>
+      <c r="D8" s="97"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28" t="s">
         <v>31</v>
@@ -5624,14 +5620,12 @@
         <v>1.3</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9" s="30">
         <v>1</v>
       </c>
-      <c r="D9" s="96">
-        <v>4.5</v>
-      </c>
+      <c r="D9" s="96"/>
       <c r="E9" s="31"/>
       <c r="F9" s="28" t="s">
         <v>31</v>
@@ -5648,7 +5642,7 @@
       </c>
       <c r="D10" s="113">
         <f>(C7*D7+C8*D8+C9*D9)/SUM(C7:C9)</f>
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="E10" s="33"/>
       <c r="F10" s="34"/>
@@ -5659,7 +5653,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="195" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="196"/>
       <c r="D11" s="196"/>
@@ -5672,14 +5666,12 @@
         <v>2.1</v>
       </c>
       <c r="B12" s="64" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="98">
         <v>0.5</v>
       </c>
-      <c r="D12" s="97">
-        <v>4</v>
-      </c>
+      <c r="D12" s="97"/>
       <c r="E12" s="27"/>
       <c r="F12" s="28" t="s">
         <v>31</v>
@@ -5691,15 +5683,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="65">
         <f>2-C12</f>
         <v>1.5</v>
       </c>
-      <c r="D13" s="96">
-        <v>4</v>
-      </c>
+      <c r="D13" s="96"/>
       <c r="E13" s="31"/>
       <c r="F13" s="28" t="s">
         <v>31</v>
@@ -5711,14 +5701,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="C14" s="66">
-        <v>2</v>
-      </c>
-      <c r="D14" s="96">
-        <v>4</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D14" s="96"/>
       <c r="E14" s="31"/>
       <c r="F14" s="28" t="s">
         <v>31</v>
@@ -5735,9 +5723,7 @@
       <c r="C15" s="30">
         <v>1</v>
       </c>
-      <c r="D15" s="96">
-        <v>4</v>
-      </c>
+      <c r="D15" s="96"/>
       <c r="E15" s="31"/>
       <c r="F15" s="28" t="s">
         <v>31</v>
@@ -5749,14 +5735,12 @@
         <v>2.5</v>
       </c>
       <c r="B16" s="67" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C16" s="68">
         <v>1</v>
       </c>
-      <c r="D16" s="99">
-        <v>4</v>
-      </c>
+      <c r="D16" s="99"/>
       <c r="E16" s="69"/>
       <c r="F16" s="70"/>
       <c r="G16" s="135"/>
@@ -5764,14 +5748,14 @@
     <row r="17" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="84"/>
       <c r="B17" s="111" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C17" s="112">
         <v>4</v>
       </c>
       <c r="D17" s="113">
         <f>(C12*D12+C13*D13+C14*D14+C15*D15+C16*D16)/SUM(C12:C16)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E17" s="33"/>
       <c r="F17" s="34"/>
@@ -5782,7 +5766,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="192" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C18" s="193"/>
       <c r="D18" s="193"/>
@@ -5800,9 +5784,7 @@
       <c r="C19" s="26">
         <v>4</v>
       </c>
-      <c r="D19" s="97">
-        <v>6</v>
-      </c>
+      <c r="D19" s="97"/>
       <c r="E19" s="27"/>
       <c r="F19" s="28" t="s">
         <v>31</v>
@@ -5819,9 +5801,7 @@
       <c r="C20" s="30">
         <v>1</v>
       </c>
-      <c r="D20" s="96">
-        <v>4</v>
-      </c>
+      <c r="D20" s="96"/>
       <c r="E20" s="31"/>
       <c r="F20" s="28" t="s">
         <v>31</v>
@@ -5840,9 +5820,7 @@
       <c r="C21" s="42">
         <v>1</v>
       </c>
-      <c r="D21" s="100">
-        <v>3</v>
-      </c>
+      <c r="D21" s="100"/>
       <c r="E21" s="41"/>
       <c r="F21" s="28" t="s">
         <v>31</v>
@@ -5852,14 +5830,14 @@
     <row r="22" spans="1:8" s="14" customFormat="1" ht="14.25" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="104"/>
       <c r="B22" s="111" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="114">
         <v>2</v>
       </c>
       <c r="D22" s="115">
         <f>(C19*D19+C20*D20+C21*D21)/SUM(C19:C21)</f>
-        <v>5.166666666666667</v>
+        <v>0</v>
       </c>
       <c r="E22" s="43"/>
       <c r="F22" s="44"/>
@@ -5870,7 +5848,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="198" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" s="199"/>
       <c r="D23" s="199"/>
@@ -5884,14 +5862,12 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" s="125">
         <v>1</v>
       </c>
-      <c r="D24" s="96">
-        <v>4</v>
-      </c>
+      <c r="D24" s="96"/>
       <c r="E24" s="39"/>
       <c r="F24" s="28" t="s">
         <v>31</v>
@@ -5904,15 +5880,13 @@
         <v>4.2</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C25" s="124">
         <f>2-C24</f>
         <v>1</v>
       </c>
-      <c r="D25" s="97">
-        <v>3</v>
-      </c>
+      <c r="D25" s="97"/>
       <c r="E25" s="40"/>
       <c r="F25" s="28" t="s">
         <v>31</v>
@@ -5929,9 +5903,7 @@
       <c r="C26" s="126">
         <v>1</v>
       </c>
-      <c r="D26" s="100">
-        <v>4</v>
-      </c>
+      <c r="D26" s="100"/>
       <c r="E26" s="41"/>
       <c r="F26" s="28" t="s">
         <v>31</v>
@@ -5948,7 +5920,7 @@
       </c>
       <c r="D27" s="115">
         <f>(C24*D24+C25*D25+C26*D26)/SUM(C24:C26)</f>
-        <v>3.6666666666666665</v>
+        <v>0</v>
       </c>
       <c r="E27" s="43"/>
       <c r="F27" s="44"/>
@@ -5962,7 +5934,7 @@
       <c r="C28" s="118"/>
       <c r="D28" s="119">
         <f>(C10*D10+C17*D17+C22*D22+C27*D27)/SUM(C10,C17,C22,C27)</f>
-        <v>4.3</v>
+        <v>0</v>
       </c>
       <c r="E28" s="45"/>
       <c r="F28" s="46"/>
@@ -5987,7 +5959,7 @@
         <v>7</v>
       </c>
       <c r="C30" s="188">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D30" s="189"/>
       <c r="E30" s="92"/>
@@ -6004,7 +5976,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="188">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D31" s="189"/>
       <c r="E31" s="93"/>
@@ -6019,7 +5991,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="190">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D32" s="191"/>
       <c r="E32" s="94"/>
@@ -6035,7 +6007,7 @@
       </c>
       <c r="C33" s="184">
         <f>0.25*SUM(C30:D32)/30</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="D33" s="185"/>
       <c r="E33" s="8"/>
@@ -6045,11 +6017,11 @@
     <row r="34" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="86"/>
       <c r="B34" s="109" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C34" s="186">
         <f>ROUND(D28+C33,1)</f>
-        <v>4.4000000000000004</v>
+        <v>0</v>
       </c>
       <c r="D34" s="187"/>
       <c r="E34" s="47"/>
@@ -6130,15 +6102,15 @@
   <sheetData>
     <row r="3" spans="1:2" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A3" s="140" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A6" s="143" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" s="144" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
@@ -6146,10 +6118,10 @@
     </row>
     <row r="8" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A8" s="143" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" s="144" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="13.5" x14ac:dyDescent="0.35">
@@ -6157,10 +6129,10 @@
     </row>
     <row r="10" spans="1:2" ht="13.9" x14ac:dyDescent="0.35">
       <c r="A10" s="145" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="146" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" s="146" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="13.15" x14ac:dyDescent="0.35">
@@ -6170,7 +6142,7 @@
     <row r="12" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A12" s="149"/>
       <c r="B12" s="148" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -6180,7 +6152,7 @@
     <row r="14" spans="1:2" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A14" s="149"/>
       <c r="B14" s="148" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -6190,7 +6162,7 @@
     <row r="16" spans="1:2" ht="38.25" x14ac:dyDescent="0.35">
       <c r="A16" s="149"/>
       <c r="B16" s="148" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -6200,7 +6172,7 @@
     <row r="18" spans="1:2" ht="51" x14ac:dyDescent="0.35">
       <c r="A18" s="151"/>
       <c r="B18" s="152" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>